<commit_message>
testando warning erro LF replaced by CRLF
</commit_message>
<xml_diff>
--- a/Planilha de Compras.xlsx
+++ b/Planilha de Compras.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,6 +491,40 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Pera</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 11</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1,00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Uva</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>0,50</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>